<commit_message>
I am working on fixing the unit test errors. Here's what I've done so far:
- I fixed the missing fields in the Book struct initialization.
- I fixed the missing argument in the Book::write_file function call.
- I removed an unused import in cell.rs.
</commit_message>
<xml_diff>
--- a/test_style.xlsx
+++ b/test_style.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Styled Sheet"/>
+    <sheet name="Styled Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0" count="0">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0">
   <si>
     <t>Hello, Styled World!</t>
   </si>
@@ -60,27 +60,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" fontId="0" borderId="0"/>
+    <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fillId="0" borderId="0" xfId="0" fontId="0"/>
-    <xf fontId="1" fillId="2" numFmtId="0" applyFont="1" borderId="0" applyFill="1"/>
-    <xf applyFill="1" numFmtId="0" fillId="3" fontId="2" applyFont="1" borderId="0"/>
+    <xf numFmtId="0" fillId="0" borderId="0" fontId="0" xfId="0"/>
+    <xf fontId="1" fillId="2" numFmtId="0" borderId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" borderId="0" fillId="3" applyFont="1" numFmtId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" xfId="0" name="Normal"/>
+    <cellStyle name="Normal" builtinId="0" xfId="0"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c s="2" r="B1" t="s">
+      <c t="s" s="2" r="B1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I will fix unit test errors due to type mismatches.
First, I will fix `Book::new` calls in `test_book.rs`, `test_cell.rs`, and `test_sheet.rs` to pass `&str` instead of `String`.
</commit_message>
<xml_diff>
--- a/test_style.xlsx
+++ b/test_style.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheets>
-    <sheet name="Styled Sheet" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Styled Sheet"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0" count="0">
   <si>
     <t>Hello, Styled World!</t>
   </si>
@@ -60,15 +60,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
+    <xf fontId="0" numFmtId="0" borderId="0" fillId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fillId="0" borderId="0" fontId="0" xfId="0"/>
-    <xf fontId="1" fillId="2" numFmtId="0" borderId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="2" borderId="0" fillId="3" applyFont="1" numFmtId="0" applyFill="1"/>
+    <xf fontId="0" numFmtId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" applyFill="1" numFmtId="0" fillId="2" fontId="1"/>
+    <xf applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" builtinId="0" xfId="0"/>
+    <cellStyle builtinId="0" xfId="0" name="Normal"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -77,7 +77,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c s="1" r="A1" t="s">
         <v>0</v>
       </c>
       <c t="s" s="2" r="B1">

</xml_diff>